<commit_message>
Created test script for new module name called Opportunities using POM structure, TestNG and DDT
</commit_message>
<xml_diff>
--- a/src/test/resources/Home.xlsx
+++ b/src/test/resources/Home.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prajw\eclipse-workspace2\VTigerCRM\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4246E810-3B37-4C7B-8CAA-83125F15B8FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A3DD7F8-4E97-4C49-9A5F-BC2AF983CBAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6840" yWindow="4776" windowWidth="7620" windowHeight="12960" activeTab="1" xr2:uid="{1D0A5637-2734-4683-BA22-E476725F1985}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{1D0A5637-2734-4683-BA22-E476725F1985}"/>
   </bookViews>
   <sheets>
     <sheet name="Contact02" sheetId="1" r:id="rId1"/>
     <sheet name="LEAD" sheetId="3" r:id="rId2"/>
-    <sheet name="Organization02" sheetId="2" r:id="rId3"/>
+    <sheet name="Opportunity" sheetId="4" r:id="rId3"/>
+    <sheet name="Organization02" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="64">
   <si>
     <t>firstname</t>
   </si>
@@ -180,13 +181,52 @@
   </si>
   <si>
     <t>Editing Lead Information</t>
+  </si>
+  <si>
+    <t>Opportunity Name</t>
+  </si>
+  <si>
+    <t>QA Engineer</t>
+  </si>
+  <si>
+    <t>Related To</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Existing Business</t>
+  </si>
+  <si>
+    <t>Lead Source</t>
+  </si>
+  <si>
+    <t>Existing Customer</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Sales Stage</t>
+  </si>
+  <si>
+    <t>Value Proposition</t>
+  </si>
+  <si>
+    <t>Probability</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Demo purpose</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -216,6 +256,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -238,7 +284,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -249,6 +295,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -672,7 +719,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EBF358B-EBBD-4EEA-9807-912D42BE07AC}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -771,6 +818,89 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E4D2C2C-E129-416C-A882-C32DC2357EF4}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="33.21875" customWidth="1"/>
+    <col min="2" max="2" width="35.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49AFB446-453F-4EBD-AF03-7DD1BA9DC8C0}">
   <dimension ref="A1:B19"/>
   <sheetViews>

</xml_diff>